<commit_message>
Fix display of check no / reciept no
</commit_message>
<xml_diff>
--- a/application/controllers/Reports.xlsx
+++ b/application/controllers/Reports.xlsx
@@ -15,7 +15,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+  <si>
+    <t>PROGEN Dieseltech Services Corp.</t>
+  </si>
+  <si>
+    <t>Purok San Jose, Brgy. Calumangan, Bago City</t>
+  </si>
+  <si>
+    <t>PAID BILLING REPORT</t>
+  </si>
+  <si>
+    <t>Negros Occidental, Philippines 6101</t>
+  </si>
+  <si>
+    <t>Tel. No. 476 - 7382</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,7 +403,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -395,8 +411,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:8">
       <c r="A1"/>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
add begbal in reports
</commit_message>
<xml_diff>
--- a/application/controllers/Reports.xlsx
+++ b/application/controllers/Reports.xlsx
@@ -15,23 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
-  <si>
-    <t>PROGEN Dieseltech Services Corp.</t>
-  </si>
-  <si>
-    <t>Purok San Jose, Brgy. Calumangan, Bago City</t>
-  </si>
-  <si>
-    <t>SALES BACKORDER</t>
-  </si>
-  <si>
-    <t>Negros Occidental, Philippines 6101</t>
-  </si>
-  <si>
-    <t>Tel. No. 476 - 7382</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -403,7 +387,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -411,29 +395,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:1">
       <c r="A1"/>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
add date filter in sales
</commit_message>
<xml_diff>
--- a/application/controllers/Reports.xlsx
+++ b/application/controllers/Reports.xlsx
@@ -15,7 +15,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+  <si>
+    <t>PROGEN Dieseltech Services Corp.</t>
+  </si>
+  <si>
+    <t>Purok San Jose, Brgy. Calumangan, Bago City</t>
+  </si>
+  <si>
+    <t>STOCKCARD REPORT</t>
+  </si>
+  <si>
+    <t>Negros Occidental, Philippines 6101</t>
+  </si>
+  <si>
+    <t>Tel. No. 476 - 7382</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,7 +403,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -395,8 +411,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:12">
       <c r="A1"/>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>